<commit_message>
changes in the credits
</commit_message>
<xml_diff>
--- a/test/reference_file.xlsx
+++ b/test/reference_file.xlsx
@@ -19,6 +19,22 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="aicpa_2.pdf" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="aicpa.pdf" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="auditsense_1.pdf" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="auditsense_2.pdf" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="becker_1.pdf" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="becker.pdf" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bkd_1.pdf" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bkd_2.pdf" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bkd_3.pdf" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cfma_less_priority.pdf" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cpa_academy.pdf" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delloite_1.pdf" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delloite_3.pdf" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ficpa.pdf" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="grant_thorton_1.pdf" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="grant_thorton_2.pdf" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ey_2.pdf" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delloite_2.pdf" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="intuit_4.pdf" sheetId="28" state="visible" r:id="rId28"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -26,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143">
   <si>
     <t>name</t>
   </si>
@@ -37,28 +53,25 @@
     <t>program_name</t>
   </si>
   <si>
-    <t>Vader and bs virtue ob the provisions of the betives of cho Associinon of Cer tiied</t>
-  </si>
-  <si>
-    <t>field_of_study</t>
-  </si>
-  <si>
-    <t>Spectahzed Knowledge</t>
+    <t>New Ways to Prevent and Detect Fraud Risks Across Employee Spend Areas tedeb tlite</t>
   </si>
   <si>
     <t>credits</t>
   </si>
   <si>
+    <t xml:space="preserve"> This participation is hereby recommended for 1.20</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
-    <t>07/12/2018</t>
+    <t>03/19/2019</t>
   </si>
   <si>
     <t>delivery_method</t>
   </si>
   <si>
-    <t>Group Internet based</t>
+    <t>Group Internet Based</t>
   </si>
   <si>
     <t>sponsor</t>
@@ -67,16 +80,25 @@
     <t>sponsor_id</t>
   </si>
   <si>
+    <t>[]</t>
+  </si>
+  <si>
     <t>qas_number</t>
   </si>
   <si>
     <t>fos</t>
   </si>
   <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>[{'name': 'Fraud', 'credits': '1.20', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>David F. McCormick CA-017896-L</t>
+  </si>
+  <si>
+    <t>"Procurement Fraud Indicators and Current Trends”</t>
+  </si>
+  <si>
+    <t>1.0</t>
   </si>
   <si>
     <t>01/16/2018</t>
@@ -88,6 +110,9 @@
     <t>Association of Certified Fraud Examiners</t>
   </si>
   <si>
+    <t>[{'name': 'Fraud', 'credits': '1.0', 'score': ''}]</t>
+  </si>
+  <si>
     <t>Fraud &amp; Embezzlement: Lessons from the Trenches Fraudulent Confessions of An Accountant Fraud Risk Management &amp; COSO: Past, Present, and Future</t>
   </si>
   <si>
@@ -97,22 +122,40 @@
     <t>Institute of Internal Auditors</t>
   </si>
   <si>
-    <t>[{'name': 'Behavioral Ethics', 'credits': '2', 'score': ''}, {'name': 'Auditing', 'credits': '4', 'score': ''}, {'name': 'Management Services', 'credits': '2', 'score': ''}]</t>
+    <t>[{'name': 'Management Services', 'credits': '2.0', 'score': ''}, {'name': 'Behavioral Ethics', 'credits': '2.0', 'score': ''}, {'name': 'Auditing', 'credits': '4.0', 'score': ''}]</t>
   </si>
   <si>
     <t>[{'name': 'Auditing'}, {'name': 'Behavioral Ethics'}, {'name': 'Management Services'}]</t>
   </si>
   <si>
-    <t>125269</t>
-  </si>
-  <si>
-    <t>Decentralized Technologies: Cryptocurrency Regulation, Anti-Money Laundering Concerns and the Importance of Knowing Your Customer hic.dl of Scudy:</t>
-  </si>
-  <si>
-    <t>08/21/2018</t>
-  </si>
-  <si>
-    <t>[{'name': 'Specialized Knowledge', 'credits': '1.20', 'score': ''}]</t>
+    <t xml:space="preserve"> 1</t>
+  </si>
+  <si>
+    <t>[{'name': 'Fraud', 'credits': '1', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>04/04/2016</t>
+  </si>
+  <si>
+    <t>Group Lve</t>
+  </si>
+  <si>
+    <t>[{'name': 'NASBA', 'id': '125269', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>[{'name': 'Fraud', 'credits': '', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Sharon Gubinsky</t>
+  </si>
+  <si>
+    <t>Decentralized Technologies: Cryptocurrency Regulation, Anti-Money Laundering Concerns and the Importance of Knowing Your Customer Fields of Study</t>
+  </si>
+  <si>
+    <t>103118</t>
+  </si>
+  <si>
+    <t>[{'name': 'Specialized Knowledge', 'credits': '1.2', 'score': ''}]</t>
   </si>
   <si>
     <t>Margaret Walsh</t>
@@ -121,19 +164,16 @@
     <t>Ethical Issues for Fraud Examiners (2013)</t>
   </si>
   <si>
-    <t>This participation is hereby recommended for 2.00</t>
-  </si>
-  <si>
-    <t>03/19/2019</t>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>01/21/2016</t>
   </si>
   <si>
     <t>QAS Self-Study</t>
   </si>
   <si>
-    <t>103118</t>
-  </si>
-  <si>
-    <t>[{'name': 'Behavioral Ethics', 'credits': '2.00', 'score': ''}]</t>
+    <t>[{'name': 'Behavioral Ethics', 'credits': '2.0', 'score': ''}]</t>
   </si>
   <si>
     <t>Juan Trezzi</t>
@@ -146,19 +186,19 @@
     <t>12/12/2015</t>
   </si>
   <si>
-    <t>10311</t>
-  </si>
-  <si>
-    <t>[{'name': 'Professional Ethics', 'credits': '1', 'score': ''}, {'name': 'Auditing', 'credits': '1.5', 'score': ''}, {'name': 'Business Law', 'credits': '8', 'score': ''}, {'name': 'Specialized Knowledge and Applications', 'credits': '15.5', 'score': ''}, {'name': 'Computer Science', 'credits': '0.5', 'score': ''}, {'name': 'Accounting', 'credits': '1.5', 'score': ''}, {'name': 'Communications', 'credits': '2', 'score': ''}]</t>
-  </si>
-  <si>
-    <t>CERTIFICATION OF COMPLETION</t>
-  </si>
-  <si>
-    <t>Tax Relief For Your Clients Federal Estate Tax and is awardedthis certificate on 1/25/20 16</t>
-  </si>
-  <si>
-    <t>01/25/2020</t>
+    <t>#1031</t>
+  </si>
+  <si>
+    <t>[{'name': 'Auditing', 'credits': '1.5', 'score': ''}, {'name': 'Computer Science', 'credits': '1.5', 'score': ''}, {'name': 'Business Law', 'credits': '8.0', 'score': ''}, {'name': 'Specialized Knowledge and Applications', 'credits': '15.5', 'score': ''}, {'name': 'Accounting', 'credits': '8.0', 'score': ''}, {'name': 'Communications', 'credits': '15.5', 'score': ''}, {'name': 'Professional Ethics', 'credits': '1.0', 'score': ''}, {'name': 'Specialized Knowledge', 'credits': '15.5', 'score': ''}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiran Bhathal </t>
+  </si>
+  <si>
+    <t>Tax Relief For Your Clients Federal Estate Tax</t>
+  </si>
+  <si>
+    <t>03/13/2019</t>
   </si>
   <si>
     <t>Internet Based Self-Study Program.</t>
@@ -176,19 +216,16 @@
     <t>[{'name': 'Taxes', 'credits': '', 'score': ''}]</t>
   </si>
   <si>
-    <t>Tammi Thomos</t>
+    <t xml:space="preserve"> Tammi Thomos</t>
   </si>
   <si>
     <t xml:space="preserve"> Free Webcast: Drive Your Competitive Edge with Audit Quality</t>
   </si>
   <si>
-    <t>03/18/0648</t>
-  </si>
-  <si>
     <t>Internet-based group-study Completion date: Tue, September 22, 2015</t>
   </si>
   <si>
-    <t>[{'name': 'Auditing', 'credits': '2', 'score': ''}]</t>
+    <t>[{'name': 'Auditing', 'credits': '2.0', 'score': ''}]</t>
   </si>
   <si>
     <t>Carmen Leung</t>
@@ -197,9 +234,6 @@
     <t>Experienced Staff</t>
   </si>
   <si>
-    <t>08/20/2022</t>
-  </si>
-  <si>
     <t>AuditSense</t>
   </si>
   <si>
@@ -207,6 +241,239 @@
   </si>
   <si>
     <t>[{'name': 'Personal Development', 'credits': '', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Zoey Hofmeister</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lease Accounting</t>
+  </si>
+  <si>
+    <t>05/01/2018</t>
+  </si>
+  <si>
+    <t>QASself study</t>
+  </si>
+  <si>
+    <t>Becker Professional Education</t>
+  </si>
+  <si>
+    <t>107294</t>
+  </si>
+  <si>
+    <t>[{'name': 'Accounting', 'credits': '30.0', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Angelica Garza</t>
+  </si>
+  <si>
+    <t>Federal Tax Update-June 2018</t>
+  </si>
+  <si>
+    <t>07/31/2018</t>
+  </si>
+  <si>
+    <t>Interactive Self Study</t>
+  </si>
+  <si>
+    <t>[{'name': 'Taxes', 'credits': '2.0', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Katelynn Stoll</t>
+  </si>
+  <si>
+    <t>What Doesthe Wayfair Ruling Mean for Your Organization? Tuesday. August 14. 2018</t>
+  </si>
+  <si>
+    <t>03/18/2018</t>
+  </si>
+  <si>
+    <t>Group Internet-Based</t>
+  </si>
+  <si>
+    <t>107848</t>
+  </si>
+  <si>
+    <t>[{'name': 'Computer Software &amp; Applications', 'credits': '0.0', 'score': ''}, {'name': 'Accounting', 'credits': '0.0', 'score': ''}, {'name': 'Business Management &amp; Organization', 'credits': '0.0', 'score': ''}, {'name': 'Economics', 'credits': '0.0', 'score': ''}, {'name': 'Regulatory Ethics', 'credits': '0.0', 'score': ''}, {'name': 'Management Services', 'credits': '0.0', 'score': ''}, {'name': 'Finance', 'credits': '0.0', 'score': ''}, {'name': 'Communications', 'credits': '0.0', 'score': ''}, {'name': 'Personal Development', 'credits': '0.0', 'score': ''}, {'name': 'Taxes', 'credits': '0.0', 'score': ''}, {'name': 'Business Law', 'credits': '0.0', 'score': ''}, {'name': 'Statistics', 'credits': '0.0', 'score': ''}, {'name': 'Behavioral Ethics', 'credits': '0.0', 'score': ''}, {'name': 'Marketing', 'credits': '0.0', 'score': ''}, {'name': 'Information Technology', 'credits': '0.0', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Jennifer Hazelton</t>
+  </si>
+  <si>
+    <t>Not-for-Profit Tax Update &amp; Introduction to 990connect Thursday. October 01. 2015</t>
+  </si>
+  <si>
+    <t>03/18/2015</t>
+  </si>
+  <si>
+    <t>[{'name': 'Behavioral Ethics', 'credits': '000', 'score': ''}, {'name': 'Statistics', 'credits': '0', 'score': ''}, {'name': 'Marketing', 'credits': '0', 'score': ''}, {'name': 'Business Law', 'credits': '000', 'score': ''}, {'name': 'Accounting', 'credits': '000', 'score': ''}, {'name': 'Communications', 'credits': '0', 'score': ''}, {'name': 'Regulatory Ethics', 'credits': '0', 'score': ''}, {'name': 'Finance', 'credits': '0', 'score': ''}, {'name': 'Social Environment of Business', 'credits': '0', 'score': ''}, {'name': 'Computer Science', 'credits': '0', 'score': ''}, {'name': 'Personal Development', 'credits': '0', 'score': ''}, {'name': 'Mathematics', 'credits': '0', 'score': ''}, {'name': 'Economics', 'credits': '0', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Tim Collman</t>
+  </si>
+  <si>
+    <t>Where Do We Go From Here? Adopting a Next-Generation Digital Mindset Tuesday. September 11. 2018</t>
+  </si>
+  <si>
+    <t>[{'name': 'Behavioral Ethics', 'credits': '000', 'score': ''}, {'name': 'Statistics', 'credits': '0', 'score': ''}, {'name': 'Marketing', 'credits': '000', 'score': ''}, {'name': 'Business Law', 'credits': '000', 'score': ''}, {'name': 'Accounting', 'credits': '000', 'score': ''}, {'name': 'Management Services', 'credits': '000', 'score': ''}, {'name': 'Communications', 'credits': '000', 'score': ''}, {'name': 'Regulatory Ethics', 'credits': '000', 'score': ''}, {'name': 'Information Technology', 'credits': '000', 'score': ''}, {'name': 'Taxes', 'credits': '0', 'score': ''}, {'name': 'Economics', 'credits': '000', 'score': ''}, {'name': 'Personal Development', 'credits': '000', 'score': ''}, {'name': 'Computer Software &amp; Applications', 'credits': '000', 'score': ''}, {'name': 'Finance', 'credits': '000', 'score': ''}, {'name': 'Business Management &amp; Organization', 'credits': '000', 'score': ''}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                         Sylvia Matlock </t>
+  </si>
+  <si>
+    <t>The Affordable Care Act: Lessons Learned and the Future of Obamacare</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>01/11/2017</t>
+  </si>
+  <si>
+    <t>1031/5</t>
+  </si>
+  <si>
+    <t>[{'name': 'Specialized Knowledge', 'credits': '1.50', 'score': ''}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Edden Burshtein</t>
+  </si>
+  <si>
+    <t>THE POWER OF PROCURE TO PAY (P2P) METRICS AND OASHBOARDS.</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>09/27/2018</t>
+  </si>
+  <si>
+    <t>Group-Intemet Based</t>
+  </si>
+  <si>
+    <t>CPA Academy</t>
+  </si>
+  <si>
+    <t>111889</t>
+  </si>
+  <si>
+    <t>[{'name': 'Business Management and Organization', 'credits': '10', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Michael Lieb</t>
+  </si>
+  <si>
+    <t>05/03/2018</t>
+  </si>
+  <si>
+    <t>Group - Internet-Based</t>
+  </si>
+  <si>
+    <t>Deloitte</t>
+  </si>
+  <si>
+    <t>[{'name': 'Specialized Knowledge', 'credits': '0', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>05/22/2018</t>
+  </si>
+  <si>
+    <t>[{'name': 'Audit', 'credits': '2018', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Robert M. Launch (682)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethics: Protecting the Integrity of Florida CPAs (4980) 
+</t>
+  </si>
+  <si>
+    <t>Ethics: 4.00</t>
+  </si>
+  <si>
+    <t>06/26/2018</t>
+  </si>
+  <si>
+    <t>Live Presentation</t>
+  </si>
+  <si>
+    <t>FICPA</t>
+  </si>
+  <si>
+    <t>[{'name': 'Regulatory Ethics', 'credits': '4.00', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>The Proposed Section 965 Regulations — Transition Tax</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>08/22/2018</t>
+  </si>
+  <si>
+    <t>Group ‘rternet basea</t>
+  </si>
+  <si>
+    <t>Grant Thornton</t>
+  </si>
+  <si>
+    <t>[{'name': 'Taxes', 'credits': '1.5', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Aimee Pourciau</t>
+  </si>
+  <si>
+    <t>Tax accounting quarterly update: September 2017 instructional Delivery Method</t>
+  </si>
+  <si>
+    <t>09/19/2017</t>
+  </si>
+  <si>
+    <t>Group Intemet Based</t>
+  </si>
+  <si>
+    <t>[{'name': 'Accounting', 'credits': '2017', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>Melissa Cook</t>
+  </si>
+  <si>
+    <t>Q2 2017 Financial Reporting Update San Jose Location: San Jose CA</t>
+  </si>
+  <si>
+    <t>06/28/2017</t>
+  </si>
+  <si>
+    <t>Self Study</t>
+  </si>
+  <si>
+    <t>[{'name': 'Accounting', 'credits': '1.5', 'score': ''}]</t>
+  </si>
+  <si>
+    <t>JEANNINE MCDONOUGH</t>
+  </si>
+  <si>
+    <t>12/14/2016</t>
+  </si>
+  <si>
+    <t>[{'name': 'Accounting', 'credits': '4', 'score': ''}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                 Module 1: Getting Started
+</t>
+  </si>
+  <si>
+    <t>7,</t>
+  </si>
+  <si>
+    <t>06/30/2016</t>
+  </si>
+  <si>
+    <t>Intuit</t>
+  </si>
+  <si>
+    <t>[{'name': 'Specialized Knowledge', 'credits': '7', 'score': ''}]</t>
   </si>
 </sst>
 </file>
@@ -573,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -581,44 +848,44 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -626,7 +893,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -634,7 +901,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -661,7 +928,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -669,17 +936,17 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -687,26 +954,26 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -714,7 +981,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -722,7 +989,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -749,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -757,59 +1024,640 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -859,20 +1707,20 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -880,15 +1728,21 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -896,7 +1750,736 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -922,39 +2505,48 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -962,17 +2554,20 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -980,7 +2575,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1015,37 +2610,40 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1059,7 +2657,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1067,7 +2665,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1101,27 +2699,30 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1134,7 +2735,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1168,33 +2769,39 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1207,7 +2814,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1233,44 +2840,50 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1283,7 +2896,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +2923,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1318,47 +2931,47 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1371,7 +2984,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1398,7 +3011,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1406,44 +3019,44 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1456,7 +3069,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>